<commit_message>
updates for first eLife revision
</commit_message>
<xml_diff>
--- a/scripts/data_prep/organize/file_names.xlsx
+++ b/scripts/data_prep/organize/file_names.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t xml:space="preserve">eye_file</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t xml:space="preserve">None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eyes_closed_rest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eyes_Closed_Rest</t>
   </si>
 </sst>
 </file>
@@ -340,10 +346,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -497,6 +503,17 @@
         <v>32</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>